<commit_message>
inner contract tmp minor fixes implemented
</commit_message>
<xml_diff>
--- a/templates/BL_New.xlsx
+++ b/templates/BL_New.xlsx
@@ -8,27 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47B3DFB-4A84-4A5F-8A57-D0608475637E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C381E7C-0567-431F-BED7-7FACE304CCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-54600" yWindow="1837" windowWidth="26865" windowHeight="15593" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BL 1 " sheetId="10" r:id="rId1"/>
+    <sheet name="BL" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BL_No">'BL 1 '!$I$3</definedName>
-    <definedName name="Bl_массив">'BL 1 '!$A$27</definedName>
-    <definedName name="Print_Are" localSheetId="0">'BL 1 '!$A$1:$I$69</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'BL 1 '!$A$1:$I$69</definedName>
-    <definedName name="Зона_вылова">'BL 1 '!$C$18</definedName>
-    <definedName name="Куда">'BL 1 '!$A$20</definedName>
-    <definedName name="Получатель">'BL 1 '!$A$8</definedName>
-    <definedName name="Получатель_адрес">'BL 1 '!$A$9</definedName>
-    <definedName name="Получатель_уведомление">'BL 1 '!$A$13</definedName>
-    <definedName name="Получатель_уведомление_адрес">'BL 1 '!$A$14</definedName>
-    <definedName name="Продавец">'BL 1 '!$A$4</definedName>
-    <definedName name="Продавец_адрес">'BL 1 '!$A$5</definedName>
-    <definedName name="Судно">'BL 1 '!$A$18</definedName>
+    <definedName name="BL_No">BL!$I$3</definedName>
+    <definedName name="Bl_массив">BL!$A$27</definedName>
+    <definedName name="Print_Are" localSheetId="0">BL!$A$1:$I$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BL!$A$1:$I$69</definedName>
+    <definedName name="Seller">BL!$A$4</definedName>
+    <definedName name="Зона_вылова">BL!$C$18</definedName>
+    <definedName name="Куда">BL!$A$20</definedName>
+    <definedName name="Получатель">BL!$A$8</definedName>
+    <definedName name="Получатель_адрес">BL!$A$9</definedName>
+    <definedName name="Получатель_уведомление">BL!$A$13</definedName>
+    <definedName name="Получатель_уведомление_адрес">BL!$A$14</definedName>
+    <definedName name="Продавец_адрес">BL!$A$5</definedName>
+    <definedName name="Судно">BL!$A$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -448,7 +448,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -600,42 +600,113 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
@@ -644,79 +715,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -999,8 +997,8 @@
   </sheetPr>
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="10.15"/>
@@ -1028,58 +1026,58 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="68" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
       <c r="I3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="69" t="s">
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
@@ -1088,119 +1086,119 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="65"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
+      <c r="A6" s="89"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="12" customHeight="1">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A10" s="56"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A11" s="56"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:12" s="87" customFormat="1" ht="12.4" customHeight="1">
-      <c r="A13" s="84" t="s">
+    <row r="13" spans="1:12" s="70" customFormat="1" ht="12.4" customHeight="1">
+      <c r="A13" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A15" s="56"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
         <v>5</v>
@@ -1210,11 +1208,11 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
+      <c r="A16" s="91"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
       <c r="F16" s="46"/>
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
@@ -1222,15 +1220,15 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58" t="s">
+      <c r="B17" s="72"/>
+      <c r="C17" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
       <c r="F17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1240,15 +1238,15 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A18" s="89" t="s">
+      <c r="A18" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="89"/>
-      <c r="C18" s="90" t="s">
+      <c r="B18" s="85"/>
+      <c r="C18" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
       <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
@@ -1258,13 +1256,13 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1272,35 +1270,35 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A20" s="88" t="s">
+      <c r="A20" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="88"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="82" t="s">
+      <c r="B20" s="83"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" ht="12" customHeight="1">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="61" t="s">
+      <c r="H21" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="61"/>
+      <c r="I21" s="73"/>
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" ht="19.899999999999999" customHeight="1">
@@ -1366,7 +1364,7 @@
       <c r="I26" s="18"/>
     </row>
     <row r="27" spans="1:12" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A27" s="96" t="s">
+      <c r="A27" s="71" t="s">
         <v>69</v>
       </c>
       <c r="B27" s="16" t="s">
@@ -1435,10 +1433,10 @@
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="64" t="s">
+      <c r="F33" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="64"/>
+      <c r="G33" s="75"/>
       <c r="H33" s="36" t="s">
         <v>56</v>
       </c>
@@ -1512,14 +1510,14 @@
     </row>
     <row r="39" spans="1:14" ht="11.65" customHeight="1">
       <c r="A39" s="8"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="83"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83"/>
-      <c r="G39" s="83"/>
-      <c r="H39" s="83"/>
-      <c r="I39" s="83"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="66"/>
     </row>
     <row r="40" spans="1:14" ht="11.65" customHeight="1">
       <c r="A40" s="8"/>
@@ -1570,14 +1568,14 @@
       <c r="C43" s="45"/>
       <c r="D43" s="45"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="93" t="s">
+      <c r="F43" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="92"/>
-      <c r="H43" s="58" t="s">
+      <c r="G43" s="79"/>
+      <c r="H43" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="I43" s="58"/>
+      <c r="I43" s="72"/>
     </row>
     <row r="44" spans="1:14" ht="12" customHeight="1">
       <c r="A44" s="47" t="s">
@@ -1587,10 +1585,10 @@
       <c r="C44" s="46"/>
       <c r="D44" s="46"/>
       <c r="E44" s="49"/>
-      <c r="F44" s="94"/>
-      <c r="G44" s="95"/>
-      <c r="H44" s="91"/>
-      <c r="I44" s="91"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="74"/>
     </row>
     <row r="45" spans="1:14" ht="12" customHeight="1">
       <c r="A45" s="35"/>
@@ -1713,15 +1711,15 @@
     <row r="55" spans="1:9" ht="12" customHeight="1">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="70" t="s">
+      <c r="D55" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="E55" s="71"/>
+      <c r="E55" s="30"/>
       <c r="F55" s="30"/>
-      <c r="G55" s="72" t="s">
+      <c r="G55" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="H55" s="73"/>
+      <c r="H55" s="56"/>
       <c r="I55" s="12"/>
     </row>
     <row r="56" spans="1:9" ht="15" customHeight="1">
@@ -1763,11 +1761,11 @@
     <row r="59" spans="1:9" ht="12" customHeight="1">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
-      <c r="D59" s="78">
+      <c r="D59" s="61">
         <v>3</v>
       </c>
-      <c r="E59" s="79"/>
-      <c r="F59" s="80"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="63"/>
       <c r="G59" s="33"/>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -1775,11 +1773,11 @@
     <row r="60" spans="1:9">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
-      <c r="D60" s="78" t="s">
+      <c r="D60" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="E60" s="79"/>
-      <c r="F60" s="80"/>
+      <c r="E60" s="62"/>
+      <c r="F60" s="63"/>
       <c r="G60" s="33"/>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
@@ -1791,109 +1789,109 @@
       <c r="D61" s="33"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
-      <c r="G61" s="74" t="s">
+      <c r="G61" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="H61" s="75"/>
-      <c r="I61" s="75"/>
+      <c r="H61" s="58"/>
+      <c r="I61" s="58"/>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="6"/>
-      <c r="D62" s="76"/>
+      <c r="D62" s="59"/>
       <c r="E62" s="8"/>
-      <c r="F62" s="77"/>
-      <c r="G62" s="74"/>
-      <c r="H62" s="75"/>
-      <c r="I62" s="75"/>
+      <c r="F62" s="60"/>
+      <c r="G62" s="57"/>
+      <c r="H62" s="58"/>
+      <c r="I62" s="58"/>
     </row>
     <row r="63" spans="1:9" ht="10.15" customHeight="1">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="6"/>
-      <c r="D63" s="76"/>
+      <c r="D63" s="59"/>
       <c r="E63" s="8"/>
-      <c r="F63" s="77"/>
-      <c r="G63" s="74" t="s">
+      <c r="F63" s="60"/>
+      <c r="G63" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="H63" s="75"/>
-      <c r="I63" s="75"/>
+      <c r="H63" s="58"/>
+      <c r="I63" s="58"/>
     </row>
     <row r="64" spans="1:9" ht="10.15" customHeight="1">
-      <c r="A64" s="75" t="s">
+      <c r="A64" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B64" s="75"/>
-      <c r="C64" s="81"/>
-      <c r="D64" s="76"/>
+      <c r="B64" s="58"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="59"/>
       <c r="E64" s="8"/>
-      <c r="F64" s="77"/>
-      <c r="G64" s="74"/>
-      <c r="H64" s="75"/>
-      <c r="I64" s="75"/>
+      <c r="F64" s="60"/>
+      <c r="G64" s="57"/>
+      <c r="H64" s="58"/>
+      <c r="I64" s="58"/>
     </row>
     <row r="65" spans="1:9" ht="10.15" customHeight="1">
-      <c r="A65" s="75" t="s">
+      <c r="A65" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="75"/>
-      <c r="C65" s="81"/>
-      <c r="D65" s="76"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="64"/>
+      <c r="D65" s="59"/>
       <c r="E65" s="8"/>
-      <c r="F65" s="77"/>
-      <c r="G65" s="74"/>
-      <c r="H65" s="75"/>
-      <c r="I65" s="75"/>
+      <c r="F65" s="60"/>
+      <c r="G65" s="57"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="58"/>
     </row>
     <row r="66" spans="1:9" ht="10.15" customHeight="1">
-      <c r="A66" s="75" t="s">
+      <c r="A66" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="B66" s="75"/>
-      <c r="C66" s="81"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="64"/>
       <c r="D66" s="34"/>
       <c r="E66" s="13"/>
       <c r="F66" s="13"/>
-      <c r="G66" s="74"/>
-      <c r="H66" s="75"/>
-      <c r="I66" s="75"/>
+      <c r="G66" s="57"/>
+      <c r="H66" s="58"/>
+      <c r="I66" s="58"/>
     </row>
     <row r="67" spans="1:9" ht="10.15" customHeight="1">
-      <c r="A67" s="75" t="s">
+      <c r="A67" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="B67" s="75"/>
-      <c r="C67" s="81"/>
+      <c r="B67" s="58"/>
+      <c r="C67" s="64"/>
       <c r="D67" s="35"/>
       <c r="E67" s="24"/>
       <c r="F67" s="24"/>
-      <c r="G67" s="74"/>
-      <c r="H67" s="75"/>
-      <c r="I67" s="75"/>
+      <c r="G67" s="57"/>
+      <c r="H67" s="58"/>
+      <c r="I67" s="58"/>
     </row>
     <row r="68" spans="1:9" ht="10.15" customHeight="1">
-      <c r="A68" s="75" t="s">
+      <c r="A68" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B68" s="75"/>
-      <c r="C68" s="81"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="64"/>
       <c r="D68" s="25"/>
-      <c r="G68" s="74"/>
-      <c r="H68" s="75"/>
-      <c r="I68" s="75"/>
+      <c r="G68" s="57"/>
+      <c r="H68" s="58"/>
+      <c r="I68" s="58"/>
     </row>
     <row r="69" spans="1:9" ht="10.15" customHeight="1">
-      <c r="A69" s="75" t="s">
+      <c r="A69" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="B69" s="75"/>
-      <c r="C69" s="81"/>
+      <c r="B69" s="58"/>
+      <c r="C69" s="64"/>
       <c r="D69" s="25"/>
-      <c r="G69" s="59"/>
-      <c r="H69" s="60"/>
-      <c r="I69" s="60"/>
+      <c r="G69" s="76"/>
+      <c r="H69" s="77"/>
+      <c r="I69" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="26">
@@ -1908,6 +1906,9 @@
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E11"/>
+    <mergeCell ref="A14:E16"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="A20:B20"/>
@@ -1919,9 +1920,6 @@
     <mergeCell ref="H43:I44"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="G69:I69"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E11"/>
-    <mergeCell ref="A14:E16"/>
     <mergeCell ref="F43:G44"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
minor fixes to inner contract and port letter tmps added
</commit_message>
<xml_diff>
--- a/templates/BL_New.xlsx
+++ b/templates/BL_New.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C381E7C-0567-431F-BED7-7FACE304CCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7558B29-DB4B-41AE-94BC-F5114D284646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54600" yWindow="1837" windowWidth="26865" windowHeight="15593" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-54105" yWindow="2415" windowWidth="26865" windowHeight="15592" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="10" r:id="rId1"/>
@@ -18,15 +18,14 @@
   <definedNames>
     <definedName name="BL_No">BL!$I$3</definedName>
     <definedName name="Bl_массив">BL!$A$27</definedName>
-    <definedName name="Print_Are" localSheetId="0">BL!$A$1:$I$69</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">BL!$A$1:$I$69</definedName>
-    <definedName name="Seller">BL!$A$4</definedName>
     <definedName name="Зона_вылова">BL!$C$18</definedName>
     <definedName name="Куда">BL!$A$20</definedName>
     <definedName name="Получатель">BL!$A$8</definedName>
     <definedName name="Получатель_адрес">BL!$A$9</definedName>
     <definedName name="Получатель_уведомление">BL!$A$13</definedName>
     <definedName name="Получатель_уведомление_адрес">BL!$A$14</definedName>
+    <definedName name="Продавец">BL!$A$4</definedName>
     <definedName name="Продавец_адрес">BL!$A$5</definedName>
     <definedName name="Судно">BL!$A$18</definedName>
   </definedNames>
@@ -647,9 +646,48 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -676,45 +714,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -997,8 +996,8 @@
   </sheetPr>
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="10.15"/>
@@ -1026,58 +1025,58 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="93" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
       <c r="I3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="94" t="s">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
@@ -1086,82 +1085,82 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="89"/>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="12" customHeight="1">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
-      <c r="A8" s="90" t="s">
+      <c r="A8" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="90"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A10" s="88"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A11" s="88"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1181,24 +1180,24 @@
       <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A15" s="88"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
         <v>5</v>
@@ -1208,11 +1207,11 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A16" s="91"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
       <c r="F16" s="46"/>
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
@@ -1220,15 +1219,15 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A17" s="72" t="s">
+      <c r="A17" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="72"/>
-      <c r="C17" s="72" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
       <c r="F17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1238,15 +1237,15 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A18" s="85" t="s">
+      <c r="A18" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="85"/>
-      <c r="C18" s="86" t="s">
+      <c r="B18" s="84"/>
+      <c r="C18" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
       <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
@@ -1256,13 +1255,13 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A19" s="72" t="s">
+      <c r="A19" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1270,13 +1269,13 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A20" s="83" t="s">
+      <c r="A20" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="83"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="83"/>
       <c r="F20" s="65" t="s">
         <v>5</v>
       </c>
@@ -1286,19 +1285,19 @@
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" ht="12" customHeight="1">
-      <c r="A21" s="72" t="s">
+      <c r="A21" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="73" t="s">
+      <c r="H21" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="73"/>
+      <c r="I21" s="86"/>
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" ht="19.899999999999999" customHeight="1">
@@ -1433,10 +1432,10 @@
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="75" t="s">
+      <c r="F33" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="75"/>
+      <c r="G33" s="88"/>
       <c r="H33" s="36" t="s">
         <v>56</v>
       </c>
@@ -1568,14 +1567,14 @@
       <c r="C43" s="45"/>
       <c r="D43" s="45"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="78" t="s">
+      <c r="F43" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="79"/>
-      <c r="H43" s="72" t="s">
+      <c r="G43" s="92"/>
+      <c r="H43" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="I43" s="72"/>
+      <c r="I43" s="77"/>
     </row>
     <row r="44" spans="1:14" ht="12" customHeight="1">
       <c r="A44" s="47" t="s">
@@ -1585,10 +1584,10 @@
       <c r="C44" s="46"/>
       <c r="D44" s="46"/>
       <c r="E44" s="49"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="81"/>
-      <c r="H44" s="74"/>
-      <c r="I44" s="74"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="87"/>
+      <c r="I44" s="87"/>
     </row>
     <row r="45" spans="1:14" ht="12" customHeight="1">
       <c r="A45" s="35"/>
@@ -1889,17 +1888,24 @@
       <c r="B69" s="58"/>
       <c r="C69" s="64"/>
       <c r="D69" s="25"/>
-      <c r="G69" s="76"/>
-      <c r="H69" s="77"/>
-      <c r="I69" s="77"/>
+      <c r="G69" s="89"/>
+      <c r="H69" s="90"/>
+      <c r="I69" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H43:I44"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="F43:G44"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:E17"/>
@@ -1909,18 +1915,11 @@
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A9:E11"/>
     <mergeCell ref="A14:E16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H43:I44"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="G69:I69"/>
-    <mergeCell ref="F43:G44"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.59055118110236227" bottom="0.19685039370078741" header="0" footer="0"/>

</xml_diff>

<commit_message>
beta new bl tmp implemented
</commit_message>
<xml_diff>
--- a/templates/BL_New.xlsx
+++ b/templates/BL_New.xlsx
@@ -8,19 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7558B29-DB4B-41AE-94BC-F5114D284646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8D6AD3-BE30-4D69-BC42-A9420BA32CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54105" yWindow="2415" windowWidth="26865" windowHeight="15592" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="At_the_port_merge_end">BL!$I$44</definedName>
+    <definedName name="At_the_port_merge_start">BL!$H$43</definedName>
     <definedName name="BL_No">BL!$I$3</definedName>
     <definedName name="Bl_массив">BL!$A$27</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">BL!$A$1:$I$69</definedName>
+    <definedName name="Shipped_merge_end">BL!$G$44</definedName>
+    <definedName name="Shipped_merge_start">BL!$F$43</definedName>
     <definedName name="Зона_вылова">BL!$C$18</definedName>
     <definedName name="Куда">BL!$A$20</definedName>
+    <definedName name="Место_дата">BL!$G$56</definedName>
     <definedName name="Получатель">BL!$A$8</definedName>
     <definedName name="Получатель_адрес">BL!$A$9</definedName>
     <definedName name="Получатель_уведомление">BL!$A$13</definedName>
@@ -47,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>Page 2</t>
   </si>
@@ -257,6 +262,9 @@
   </si>
   <si>
     <t>17 416      CARTOONS</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -646,6 +654,18 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
@@ -692,9 +712,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -704,15 +721,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -996,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="10.15"/>
@@ -1025,58 +1033,58 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="74" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
       <c r="I3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="76" t="s">
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
@@ -1085,82 +1093,82 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="78"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="12" customHeight="1">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1180,24 +1188,24 @@
       <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A15" s="75"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
+      <c r="A15" s="79"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
         <v>5</v>
@@ -1207,11 +1215,11 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A16" s="80"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="84"/>
       <c r="F16" s="46"/>
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
@@ -1219,15 +1227,15 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77" t="s">
+      <c r="B17" s="81"/>
+      <c r="C17" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
       <c r="F17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1237,15 +1245,15 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A18" s="84" t="s">
+      <c r="A18" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="84"/>
-      <c r="C18" s="85" t="s">
+      <c r="B18" s="88"/>
+      <c r="C18" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
       <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
@@ -1255,13 +1263,13 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1269,13 +1277,13 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A20" s="82" t="s">
+      <c r="A20" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="82"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="83"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
       <c r="F20" s="65" t="s">
         <v>5</v>
       </c>
@@ -1285,19 +1293,19 @@
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" ht="12" customHeight="1">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="86" t="s">
+      <c r="H21" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="86"/>
+      <c r="I21" s="90"/>
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" ht="19.899999999999999" customHeight="1">
@@ -1432,10 +1440,10 @@
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="88" t="s">
+      <c r="F33" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="88"/>
+      <c r="G33" s="91"/>
       <c r="H33" s="36" t="s">
         <v>56</v>
       </c>
@@ -1567,14 +1575,14 @@
       <c r="C43" s="45"/>
       <c r="D43" s="45"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="91" t="s">
+      <c r="F43" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="92"/>
-      <c r="H43" s="77" t="s">
+      <c r="G43" s="73"/>
+      <c r="H43" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="I43" s="77"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:14" ht="12" customHeight="1">
       <c r="A44" s="47" t="s">
@@ -1584,10 +1592,14 @@
       <c r="C44" s="46"/>
       <c r="D44" s="46"/>
       <c r="E44" s="49"/>
-      <c r="F44" s="93"/>
-      <c r="G44" s="94"/>
-      <c r="H44" s="87"/>
-      <c r="I44" s="87"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="45" spans="1:14" ht="12" customHeight="1">
       <c r="A45" s="35"/>
@@ -1624,7 +1636,6 @@
       <c r="F47" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="G47" s="37"/>
       <c r="H47" s="37"/>
       <c r="I47" s="37"/>
     </row>
@@ -1888,18 +1899,16 @@
       <c r="B69" s="58"/>
       <c r="C69" s="64"/>
       <c r="D69" s="25"/>
-      <c r="G69" s="89"/>
-      <c r="H69" s="90"/>
-      <c r="I69" s="90"/>
+      <c r="G69" s="92"/>
+      <c r="H69" s="93"/>
+      <c r="I69" s="93"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="24">
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H43:I44"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="G69:I69"/>
-    <mergeCell ref="F43:G44"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="A20:B20"/>

</xml_diff>

<commit_message>
port letter tmp cargo fixed (empty cell fn bug) + removed date input in export cfr section
</commit_message>
<xml_diff>
--- a/templates/BL_New.xlsx
+++ b/templates/BL_New.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8D6AD3-BE30-4D69-BC42-A9420BA32CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F5D6BB-8C9F-4031-869A-F51C155EC458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="10" r:id="rId1"/>
@@ -666,62 +666,62 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1004,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="10.15"/>
@@ -1016,9 +1016,9 @@
     <col min="4" max="4" width="13.375" style="2" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" customWidth="1"/>
     <col min="6" max="6" width="7.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.3125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.4375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.0625" style="3" customWidth="1"/>
     <col min="10" max="10" width="8.75" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="2"/>
     <col min="12" max="12" width="7.375" style="2" bestFit="1" customWidth="1"/>
@@ -1033,58 +1033,58 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="78" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
       <c r="I3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="80" t="s">
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
@@ -1093,82 +1093,82 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="82"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
+      <c r="A6" s="90"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="12" customHeight="1">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A10" s="79"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A11" s="79"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1188,24 +1188,24 @@
       <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A15" s="79"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
         <v>5</v>
@@ -1215,11 +1215,11 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A16" s="84"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="84"/>
+      <c r="A16" s="89"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
       <c r="F16" s="46"/>
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
@@ -1227,15 +1227,15 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
       <c r="F17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1245,15 +1245,15 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="88"/>
-      <c r="C18" s="89" t="s">
+      <c r="B18" s="85"/>
+      <c r="C18" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
       <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
@@ -1263,13 +1263,13 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1277,13 +1277,13 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="86"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
       <c r="F20" s="65" t="s">
         <v>5</v>
       </c>
@@ -1293,19 +1293,19 @@
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" ht="12" customHeight="1">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="90" t="s">
+      <c r="H21" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="90"/>
+      <c r="I21" s="78"/>
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" ht="19.899999999999999" customHeight="1">
@@ -1440,10 +1440,10 @@
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="91" t="s">
+      <c r="F33" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="91"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="36" t="s">
         <v>56</v>
       </c>
@@ -1575,7 +1575,7 @@
       <c r="C43" s="45"/>
       <c r="D43" s="45"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="94" t="s">
+      <c r="F43" s="76" t="s">
         <v>24</v>
       </c>
       <c r="G43" s="73"/>
@@ -1899,12 +1899,28 @@
       <c r="B69" s="58"/>
       <c r="C69" s="64"/>
       <c r="D69" s="25"/>
-      <c r="G69" s="92"/>
-      <c r="H69" s="93"/>
-      <c r="I69" s="93"/>
+      <c r="G69" s="80"/>
+      <c r="H69" s="81"/>
+      <c r="I69" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E11"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A14:E16"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="F33:G33"/>
@@ -1913,25 +1929,9 @@
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E11"/>
-    <mergeCell ref="A14:E16"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.59055118110236227" bottom="0.19685039370078741" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>